<commit_message>
fixed bugs on how to read the cells
fixed letter to number conversion.
changed cellsToRead from hashmap to arraylist of int pairs(NumberTranslatedCellId class)
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">då</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lol</t>
   </si>
 </sst>
 </file>
@@ -132,13 +138,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:AAA15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ZY1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AAA14" activeCellId="0" sqref="AAA14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -153,6 +159,20 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="AAA1" s="0" t="n">
+        <f aca="false">COLUMN()</f>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AAA13" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>